<commit_message>
average for 50 runs foe all instances
average for 50 runs foe all instances
</commit_message>
<xml_diff>
--- a/Average_for_50_runs_all_instances/average_for_50_runs_all_instances_Excel.xlsx
+++ b/Average_for_50_runs_all_instances/average_for_50_runs_all_instances_Excel.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="average_for_50_runs_all_instanc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Average</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>MakeSpans for 50 iterations, MAX_ISTEPS 100000, pc=1.0, pm=0.009765625, popsize=512:</t>
+  </si>
+  <si>
+    <t>Instance</t>
   </si>
 </sst>
 </file>
@@ -349,7 +352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,8 +532,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -645,6 +654,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -690,9 +714,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1038,7 +1069,7 @@
   <dimension ref="A1:AZ15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1054,166 +1085,169 @@
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="U3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="V3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="W3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="X3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Y3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="Z3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AA3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AB3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AC3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AD3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AE3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AF3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AG3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AH3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AI3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AJ3" s="1" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AK3" s="1" t="s">
+      <c r="AK3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AL3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AM3" s="1" t="s">
+      <c r="AM3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AN3" s="1" t="s">
+      <c r="AN3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AO3" s="1" t="s">
+      <c r="AO3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AP3" s="1" t="s">
+      <c r="AP3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AQ3" s="1" t="s">
+      <c r="AQ3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AR3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AS3" s="1" t="s">
+      <c r="AS3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AT3" s="1" t="s">
+      <c r="AT3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AU3" s="1" t="s">
+      <c r="AU3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AV3" s="1" t="s">
+      <c r="AV3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AW3" s="1" t="s">
+      <c r="AW3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AX3" s="1" t="s">
+      <c r="AX3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AY3" s="1" t="s">
+      <c r="AY3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AZ3" s="1" t="s">
+      <c r="AZ3" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="1">
-        <f>AVERAGE(C4:AZ4)</f>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B15" si="0">AVERAGE(C4:AZ4)</f>
         <v>15966430.02</v>
       </c>
       <c r="C4" s="1">
@@ -1368,11 +1402,11 @@
       </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="1">
-        <f>AVERAGE(C5:AZ5)</f>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
         <v>204158.72</v>
       </c>
       <c r="C5" s="1">
@@ -1527,11 +1561,11 @@
       </c>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="1">
-        <f>AVERAGE(C6:AZ6)</f>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
         <v>529462</v>
       </c>
       <c r="C6" s="1">
@@ -1686,11 +1720,11 @@
       </c>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="1">
-        <f>AVERAGE(C7:AZ7)</f>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
         <v>6907.56</v>
       </c>
       <c r="C7" s="1">
@@ -1845,11 +1879,11 @@
       </c>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="1">
-        <f>AVERAGE(C8:AZ8)</f>
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
         <v>16662829.08</v>
       </c>
       <c r="C8" s="1">
@@ -2004,11 +2038,11 @@
       </c>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="1">
-        <f>AVERAGE(C9:AZ9)</f>
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
         <v>210435.48</v>
       </c>
       <c r="C9" s="1">
@@ -2163,11 +2197,11 @@
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="1">
-        <f>AVERAGE(C10:AZ10)</f>
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
         <v>540188.18000000005</v>
       </c>
       <c r="C10" s="1">
@@ -2322,11 +2356,11 @@
       </c>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="1">
-        <f>AVERAGE(C11:AZ11)</f>
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
         <v>7043.12</v>
       </c>
       <c r="C11" s="1">
@@ -2481,11 +2515,11 @@
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="1">
-        <f>AVERAGE(C12:AZ12)</f>
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
         <v>15757343.960000001</v>
       </c>
       <c r="C12" s="1">
@@ -2640,11 +2674,11 @@
       </c>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="1">
-        <f>AVERAGE(C13:AZ13)</f>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
         <v>203290.48</v>
       </c>
       <c r="C13" s="1">
@@ -2799,11 +2833,11 @@
       </c>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="1">
-        <f>AVERAGE(C14:AZ14)</f>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
         <v>481462.26</v>
       </c>
       <c r="C14" s="1">
@@ -2958,11 +2992,11 @@
       </c>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="1">
-        <f>AVERAGE(C15:AZ15)</f>
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
         <v>7373.58</v>
       </c>
       <c r="C15" s="1">

</xml_diff>